<commit_message>
Clustering with all database groups
</commit_message>
<xml_diff>
--- a/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
+++ b/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\Clustering_Framework\FeatureEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFF89CD-EF6F-41AD-939D-215D078B91B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2950D566-5E8D-4F53-B544-D59E5FC381A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2792A3-F0C5-48C1-A90B-69EA6F275323}"/>
   </bookViews>
@@ -264,7 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +286,13 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Bahnschrift Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Bahnschrift Light"/>
@@ -450,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -467,12 +474,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,12 +485,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -506,6 +501,21 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C7A390-9349-4E1E-BAD7-74963176F530}">
   <dimension ref="I1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,13 +930,13 @@
     </row>
     <row r="7" spans="9:20" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I7" s="4"/>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="12" t="s">
         <v>54</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="17" t="s">
+      <c r="N7" s="13" t="s">
         <v>63</v>
       </c>
       <c r="O7" s="5"/>
@@ -937,18 +947,18 @@
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="O8" s="2"/>
@@ -959,16 +969,16 @@
       <c r="T8" s="2"/>
     </row>
     <row r="9" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I9" s="12"/>
-      <c r="J9" s="13" t="s">
+      <c r="I9" s="10"/>
+      <c r="J9" s="11" t="s">
         <v>51</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="14" t="s">
         <v>65</v>
       </c>
       <c r="O9" s="2"/>
@@ -979,7 +989,7 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="9:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="19" t="s">
         <v>49</v>
       </c>
       <c r="J10" s="6" t="s">
@@ -987,7 +997,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="20" t="s">
+      <c r="M10" s="16" t="s">
         <v>66</v>
       </c>
       <c r="N10" s="6" t="s">
@@ -1001,7 +1011,7 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="19" t="s">
         <v>48</v>
       </c>
       <c r="J11" s="6" t="s">
@@ -1009,7 +1019,7 @@
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="21"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="6"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1019,7 +1029,7 @@
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="19" t="s">
         <v>47</v>
       </c>
       <c r="J12" s="6" t="s">
@@ -1027,7 +1037,7 @@
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="21"/>
+      <c r="M12" s="17"/>
       <c r="N12" s="6"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1037,7 +1047,7 @@
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="19" t="s">
         <v>46</v>
       </c>
       <c r="J13" s="6" t="s">
@@ -1045,7 +1055,7 @@
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="21"/>
+      <c r="M13" s="17"/>
       <c r="N13" s="6"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1055,7 +1065,7 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="20" t="s">
         <v>45</v>
       </c>
       <c r="J14" s="6" t="s">
@@ -1063,7 +1073,7 @@
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="21"/>
+      <c r="M14" s="17"/>
       <c r="N14" s="6"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1073,7 +1083,7 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="20" t="s">
         <v>44</v>
       </c>
       <c r="J15" s="6" t="s">
@@ -1081,7 +1091,7 @@
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="21"/>
+      <c r="M15" s="17"/>
       <c r="N15" s="6"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1091,13 +1101,13 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I16" s="12"/>
-      <c r="J16" s="13" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="11" t="s">
         <v>50</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="21"/>
+      <c r="M16" s="17"/>
       <c r="N16" s="6"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1107,7 +1117,7 @@
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="19" t="s">
         <v>43</v>
       </c>
       <c r="J17" s="6" t="s">
@@ -1115,7 +1125,7 @@
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="21"/>
+      <c r="M17" s="17"/>
       <c r="N17" s="6"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1125,7 +1135,7 @@
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="19" t="s">
         <v>42</v>
       </c>
       <c r="J18" s="6" t="s">
@@ -1133,7 +1143,7 @@
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="21"/>
+      <c r="M18" s="17"/>
       <c r="N18" s="6"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1143,7 +1153,7 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="22" t="s">
         <v>41</v>
       </c>
       <c r="J19" s="6" t="s">
@@ -1151,7 +1161,7 @@
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="21"/>
+      <c r="M19" s="17"/>
       <c r="N19" s="6"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1161,7 +1171,7 @@
       <c r="T19" s="1"/>
     </row>
     <row r="20" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="19" t="s">
         <v>38</v>
       </c>
       <c r="J20" s="6" t="s">
@@ -1169,7 +1179,7 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="21"/>
+      <c r="M20" s="17"/>
       <c r="N20" s="6"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1179,7 +1189,7 @@
       <c r="T20" s="1"/>
     </row>
     <row r="21" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="19" t="s">
         <v>39</v>
       </c>
       <c r="J21" s="6" t="s">
@@ -1187,7 +1197,7 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="21"/>
+      <c r="M21" s="17"/>
       <c r="N21" s="6"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1197,7 +1207,7 @@
       <c r="T21" s="1"/>
     </row>
     <row r="22" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="20" t="s">
         <v>40</v>
       </c>
       <c r="J22" s="6" t="s">
@@ -1205,7 +1215,7 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="21"/>
+      <c r="M22" s="17"/>
       <c r="N22" s="6"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1215,7 +1225,7 @@
       <c r="T22" s="1"/>
     </row>
     <row r="23" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I23" s="9" t="s">
+      <c r="I23" s="20" t="s">
         <v>62</v>
       </c>
       <c r="J23" s="6" t="s">
@@ -1223,7 +1233,7 @@
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="21"/>
+      <c r="M23" s="17"/>
       <c r="N23" s="6"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1233,7 +1243,7 @@
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I24" s="9" t="s">
+      <c r="I24" s="20" t="s">
         <v>37</v>
       </c>
       <c r="J24" s="6" t="s">
@@ -1241,7 +1251,7 @@
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="21"/>
+      <c r="M24" s="17"/>
       <c r="N24" s="6"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1251,7 +1261,7 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I25" s="9" t="s">
+      <c r="I25" s="20" t="s">
         <v>36</v>
       </c>
       <c r="J25" s="6" t="s">
@@ -1259,7 +1269,7 @@
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="21"/>
+      <c r="M25" s="17"/>
       <c r="N25" s="6"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1269,7 +1279,7 @@
       <c r="T25" s="1"/>
     </row>
     <row r="26" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="20" t="s">
         <v>35</v>
       </c>
       <c r="J26" s="6" t="s">
@@ -1277,7 +1287,7 @@
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="21"/>
+      <c r="M26" s="17"/>
       <c r="N26" s="6"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1287,7 +1297,7 @@
       <c r="T26" s="1"/>
     </row>
     <row r="27" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="20" t="s">
         <v>34</v>
       </c>
       <c r="J27" s="6" t="s">
@@ -1295,7 +1305,7 @@
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="21"/>
+      <c r="M27" s="17"/>
       <c r="N27" s="6"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -1305,7 +1315,7 @@
       <c r="T27" s="1"/>
     </row>
     <row r="28" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I28" s="9" t="s">
+      <c r="I28" s="20" t="s">
         <v>33</v>
       </c>
       <c r="J28" s="6" t="s">
@@ -1313,7 +1323,7 @@
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="22"/>
+      <c r="M28" s="18"/>
       <c r="N28" s="7"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1323,7 +1333,7 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="20" t="s">
         <v>32</v>
       </c>
       <c r="J29" s="6" t="s">
@@ -1341,7 +1351,7 @@
       <c r="T29" s="1"/>
     </row>
     <row r="30" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="20" t="s">
         <v>31</v>
       </c>
       <c r="J30" s="6" t="s">
@@ -1359,7 +1369,7 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="19" t="s">
         <v>30</v>
       </c>
       <c r="J31" s="6" t="s">
@@ -1377,8 +1387,8 @@
       <c r="T31" s="1"/>
     </row>
     <row r="32" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I32" s="12"/>
-      <c r="J32" s="13" t="s">
+      <c r="I32" s="21"/>
+      <c r="J32" s="11" t="s">
         <v>52</v>
       </c>
       <c r="K32" s="1"/>
@@ -1393,7 +1403,7 @@
       <c r="T32" s="1"/>
     </row>
     <row r="33" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="20" t="s">
         <v>29</v>
       </c>
       <c r="J33" s="6" t="s">
@@ -1411,7 +1421,7 @@
       <c r="T33" s="1"/>
     </row>
     <row r="34" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I34" s="9" t="s">
+      <c r="I34" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J34" s="6" t="s">
@@ -1429,7 +1439,7 @@
       <c r="T34" s="1"/>
     </row>
     <row r="35" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="20" t="s">
         <v>27</v>
       </c>
       <c r="J35" s="6" t="s">
@@ -1447,7 +1457,7 @@
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="20" t="s">
         <v>26</v>
       </c>
       <c r="J36" s="6" t="s">
@@ -1465,7 +1475,7 @@
       <c r="T36" s="1"/>
     </row>
     <row r="37" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I37" s="9" t="s">
+      <c r="I37" s="20" t="s">
         <v>25</v>
       </c>
       <c r="J37" s="6" t="s">
@@ -1483,7 +1493,7 @@
       <c r="T37" s="1"/>
     </row>
     <row r="38" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="20" t="s">
         <v>24</v>
       </c>
       <c r="J38" s="6" t="s">
@@ -1501,8 +1511,8 @@
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I39" s="12"/>
-      <c r="J39" s="13" t="s">
+      <c r="I39" s="21"/>
+      <c r="J39" s="11" t="s">
         <v>53</v>
       </c>
       <c r="K39" s="1"/>
@@ -1517,7 +1527,7 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I40" s="15" t="s">
+      <c r="I40" s="23" t="s">
         <v>23</v>
       </c>
       <c r="J40" s="7" t="s">

</xml_diff>

<commit_message>
Adding records to 'featured_records' table using Json for the features column
</commit_message>
<xml_diff>
--- a/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
+++ b/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\Clustering_Framework\FeatureEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2950D566-5E8D-4F53-B544-D59E5FC381A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98709E1A-CD89-42D2-997F-016707977365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2792A3-F0C5-48C1-A90B-69EA6F275323}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>Initials</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Average distance per figure fixation</t>
+  </si>
+  <si>
+    <t>double precision[]</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,6 +351,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -457,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -510,12 +519,13 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C7A390-9349-4E1E-BAD7-74963176F530}">
   <dimension ref="I1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I40"/>
+    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1102,9 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="6"/>
+      <c r="N15" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -1153,10 +1165,10 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="24" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="1"/>
@@ -1527,7 +1539,7 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I40" s="23" t="s">
+      <c r="I40" s="22" t="s">
         <v>23</v>
       </c>
       <c r="J40" s="7" t="s">

</xml_diff>

<commit_message>
Iterating through clustering parameters
</commit_message>
<xml_diff>
--- a/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
+++ b/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\Clustering_Framework\FeatureEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98709E1A-CD89-42D2-997F-016707977365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7826A340-1D6D-4DD3-B3FC-DD6B73337735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2792A3-F0C5-48C1-A90B-69EA6F275323}"/>
   </bookViews>
@@ -161,9 +161,6 @@
     <t>SFC</t>
   </si>
   <si>
-    <t>ASC</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>double precision[]</t>
+  </si>
+  <si>
+    <t>ASD</t>
   </si>
 </sst>
 </file>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C7A390-9349-4E1E-BAD7-74963176F530}">
   <dimension ref="I1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,13 +941,13 @@
     <row r="7" spans="9:20" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I7" s="4"/>
       <c r="J7" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -981,15 +981,15 @@
     <row r="9" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I9" s="10"/>
       <c r="J9" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N9" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>65</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
@@ -1000,18 +1000,18 @@
     </row>
     <row r="10" spans="9:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="11" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I11" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>2</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="12" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I12" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>3</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="13" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I13" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>4</v>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="14" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I14" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1094,16 +1094,16 @@
     </row>
     <row r="15" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I15" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="17"/>
       <c r="N15" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1115,7 +1115,7 @@
     <row r="16" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I16" s="21"/>
       <c r="J16" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1130,10 +1130,10 @@
     </row>
     <row r="17" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I17" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="18" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I18" s="19" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>5</v>
@@ -1223,7 +1223,7 @@
         <v>40</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1238,10 +1238,10 @@
     </row>
     <row r="23" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I23" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1385,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1401,7 +1401,7 @@
     <row r="32" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I32" s="21"/>
       <c r="J32" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1525,7 +1525,7 @@
     <row r="39" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I39" s="21"/>
       <c r="J39" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>

</xml_diff>

<commit_message>
Event detection with EMA working relatively fine. (code needs refactoring)
</commit_message>
<xml_diff>
--- a/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
+++ b/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\Clustering_Framework\FeatureEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7826A340-1D6D-4DD3-B3FC-DD6B73337735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5174387-6413-49AD-9FAB-53C577AAD280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2792A3-F0C5-48C1-A90B-69EA6F275323}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>Initials</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t>Average distance per figure fixation</t>
-  </si>
-  <si>
-    <t>double precision[]</t>
   </si>
   <si>
     <t>ASD</t>
@@ -329,12 +326,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -357,6 +348,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -466,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -489,16 +486,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -510,18 +507,19 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -842,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C7A390-9349-4E1E-BAD7-74963176F530}">
   <dimension ref="I1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M9" activeCellId="7" sqref="I10:I13 I15 I17:I18 I20:I21 I23 I25:I27 I40 M9:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,10 +1073,10 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="23" t="s">
         <v>57</v>
       </c>
       <c r="K14" s="1"/>
@@ -1093,7 +1091,7 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>43</v>
       </c>
       <c r="J15" s="6" t="s">
@@ -1102,9 +1100,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="N15" s="6"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -1113,7 +1109,7 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I16" s="21"/>
+      <c r="I16" s="20"/>
       <c r="J16" s="11" t="s">
         <v>49</v>
       </c>
@@ -1148,7 +1144,7 @@
     </row>
     <row r="18" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I18" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>5</v>
@@ -1165,10 +1161,10 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="23" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="1"/>
@@ -1219,10 +1215,10 @@
       <c r="T21" s="1"/>
     </row>
     <row r="22" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="23" t="s">
         <v>54</v>
       </c>
       <c r="K22" s="1"/>
@@ -1237,7 +1233,7 @@
       <c r="T22" s="1"/>
     </row>
     <row r="23" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="19" t="s">
         <v>61</v>
       </c>
       <c r="J23" s="6" t="s">
@@ -1255,10 +1251,10 @@
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="23" t="s">
         <v>9</v>
       </c>
       <c r="K24" s="1"/>
@@ -1273,7 +1269,7 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="19" t="s">
         <v>36</v>
       </c>
       <c r="J25" s="6" t="s">
@@ -1291,7 +1287,7 @@
       <c r="T25" s="1"/>
     </row>
     <row r="26" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I26" s="20" t="s">
+      <c r="I26" s="19" t="s">
         <v>35</v>
       </c>
       <c r="J26" s="6" t="s">
@@ -1309,7 +1305,7 @@
       <c r="T26" s="1"/>
     </row>
     <row r="27" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I27" s="20" t="s">
+      <c r="I27" s="19" t="s">
         <v>34</v>
       </c>
       <c r="J27" s="6" t="s">
@@ -1327,10 +1323,10 @@
       <c r="T27" s="1"/>
     </row>
     <row r="28" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I28" s="20" t="s">
+      <c r="I28" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="J28" s="23" t="s">
         <v>13</v>
       </c>
       <c r="K28" s="1"/>
@@ -1345,10 +1341,10 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I29" s="20" t="s">
+      <c r="I29" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="J29" s="23" t="s">
         <v>14</v>
       </c>
       <c r="K29" s="1"/>
@@ -1363,10 +1359,10 @@
       <c r="T29" s="1"/>
     </row>
     <row r="30" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I30" s="20" t="s">
+      <c r="I30" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="J30" s="23" t="s">
         <v>15</v>
       </c>
       <c r="K30" s="1"/>
@@ -1381,10 +1377,10 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I31" s="19" t="s">
+      <c r="I31" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J31" s="23" t="s">
         <v>55</v>
       </c>
       <c r="K31" s="1"/>
@@ -1399,7 +1395,7 @@
       <c r="T31" s="1"/>
     </row>
     <row r="32" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I32" s="21"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="11" t="s">
         <v>51</v>
       </c>
@@ -1415,10 +1411,10 @@
       <c r="T32" s="1"/>
     </row>
     <row r="33" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I33" s="20" t="s">
+      <c r="I33" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="J33" s="25" t="s">
         <v>16</v>
       </c>
       <c r="K33" s="1"/>
@@ -1433,10 +1429,10 @@
       <c r="T33" s="1"/>
     </row>
     <row r="34" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I34" s="20" t="s">
+      <c r="I34" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="J34" s="25" t="s">
         <v>17</v>
       </c>
       <c r="K34" s="1"/>
@@ -1451,10 +1447,10 @@
       <c r="T34" s="1"/>
     </row>
     <row r="35" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I35" s="20" t="s">
+      <c r="I35" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="J35" s="25" t="s">
         <v>18</v>
       </c>
       <c r="K35" s="1"/>
@@ -1469,10 +1465,10 @@
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I36" s="20" t="s">
+      <c r="I36" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="25" t="s">
         <v>19</v>
       </c>
       <c r="K36" s="1"/>
@@ -1487,10 +1483,10 @@
       <c r="T36" s="1"/>
     </row>
     <row r="37" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I37" s="20" t="s">
+      <c r="I37" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J37" s="6" t="s">
+      <c r="J37" s="25" t="s">
         <v>20</v>
       </c>
       <c r="K37" s="1"/>
@@ -1505,10 +1501,10 @@
       <c r="T37" s="1"/>
     </row>
     <row r="38" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I38" s="20" t="s">
+      <c r="I38" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="6" t="s">
+      <c r="J38" s="25" t="s">
         <v>21</v>
       </c>
       <c r="K38" s="1"/>
@@ -1523,7 +1519,7 @@
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I39" s="21"/>
+      <c r="I39" s="20"/>
       <c r="J39" s="11" t="s">
         <v>52</v>
       </c>
@@ -1539,7 +1535,7 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I40" s="22" t="s">
+      <c r="I40" s="21" t="s">
         <v>23</v>
       </c>
       <c r="J40" s="7" t="s">

</xml_diff>

<commit_message>
Analyzing results with Scattered data using PCA | Building decision trees for data visualization
</commit_message>
<xml_diff>
--- a/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
+++ b/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\Clustering_Framework\FeatureEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5174387-6413-49AD-9FAB-53C577AAD280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D928030B-B48E-407A-BB0B-5563B7BEE37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2792A3-F0C5-48C1-A90B-69EA6F275323}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Initials</t>
   </si>
@@ -258,6 +259,24 @@
   </si>
   <si>
     <t>ASD</t>
+  </si>
+  <si>
+    <t>Average distance to target during fixation</t>
+  </si>
+  <si>
+    <t>ADTF</t>
+  </si>
+  <si>
+    <t>ADB</t>
+  </si>
+  <si>
+    <t>ADBF</t>
+  </si>
+  <si>
+    <t>Average distance between eyes</t>
+  </si>
+  <si>
+    <t>Average distance between eyes during fixations</t>
   </si>
 </sst>
 </file>
@@ -320,12 +339,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -354,6 +367,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -463,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -486,44 +505,45 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C7A390-9349-4E1E-BAD7-74963176F530}">
   <dimension ref="I1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" activeCellId="7" sqref="I10:I13 I15 I17:I18 I20:I21 I23 I25:I27 I40 M9:M10"/>
+    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +869,7 @@
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="99.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="51.42578125" customWidth="1"/>
+    <col min="14" max="14" width="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
@@ -983,7 +1003,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="25" t="s">
         <v>63</v>
       </c>
       <c r="N9" s="14" t="s">
@@ -997,7 +1017,7 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="9:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="17" t="s">
         <v>48</v>
       </c>
       <c r="J10" s="6" t="s">
@@ -1005,7 +1025,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="24" t="s">
         <v>65</v>
       </c>
       <c r="N10" s="6" t="s">
@@ -1019,7 +1039,7 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="17" t="s">
         <v>47</v>
       </c>
       <c r="J11" s="6" t="s">
@@ -1027,8 +1047,12 @@
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="6"/>
+      <c r="M11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -1037,7 +1061,7 @@
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="17" t="s">
         <v>46</v>
       </c>
       <c r="J12" s="6" t="s">
@@ -1045,8 +1069,12 @@
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="6"/>
+      <c r="M12" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -1055,7 +1083,7 @@
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="17" t="s">
         <v>45</v>
       </c>
       <c r="J13" s="6" t="s">
@@ -1063,8 +1091,12 @@
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="6"/>
+      <c r="M13" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -1073,15 +1105,15 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="21" t="s">
         <v>57</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="17"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="6"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1091,7 +1123,7 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J15" s="6" t="s">
@@ -1099,7 +1131,7 @@
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="17"/>
+      <c r="M15" s="15"/>
       <c r="N15" s="6"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1109,13 +1141,13 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I16" s="20"/>
+      <c r="I16" s="18"/>
       <c r="J16" s="11" t="s">
         <v>49</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="17"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="6"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1125,7 +1157,7 @@
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="17" t="s">
         <v>42</v>
       </c>
       <c r="J17" s="6" t="s">
@@ -1133,7 +1165,7 @@
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="17"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="6"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1143,7 +1175,7 @@
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="17" t="s">
         <v>67</v>
       </c>
       <c r="J18" s="6" t="s">
@@ -1151,7 +1183,7 @@
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="17"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="6"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1161,15 +1193,15 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="21" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="17"/>
+      <c r="M19" s="15"/>
       <c r="N19" s="6"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1179,7 +1211,7 @@
       <c r="T19" s="1"/>
     </row>
     <row r="20" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="17" t="s">
         <v>38</v>
       </c>
       <c r="J20" s="6" t="s">
@@ -1187,7 +1219,7 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="17"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="6"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1197,7 +1229,7 @@
       <c r="T20" s="1"/>
     </row>
     <row r="21" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J21" s="6" t="s">
@@ -1205,7 +1237,7 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="17"/>
+      <c r="M21" s="15"/>
       <c r="N21" s="6"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1215,15 +1247,15 @@
       <c r="T21" s="1"/>
     </row>
     <row r="22" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I22" s="22" t="s">
+      <c r="I22" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="21" t="s">
         <v>54</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="17"/>
+      <c r="M22" s="15"/>
       <c r="N22" s="6"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1233,7 +1265,7 @@
       <c r="T22" s="1"/>
     </row>
     <row r="23" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="17" t="s">
         <v>61</v>
       </c>
       <c r="J23" s="6" t="s">
@@ -1241,7 +1273,7 @@
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="17"/>
+      <c r="M23" s="15"/>
       <c r="N23" s="6"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1251,15 +1283,15 @@
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="21" t="s">
         <v>9</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="17"/>
+      <c r="M24" s="15"/>
       <c r="N24" s="6"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1269,7 +1301,7 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I25" s="19" t="s">
+      <c r="I25" s="17" t="s">
         <v>36</v>
       </c>
       <c r="J25" s="6" t="s">
@@ -1277,7 +1309,7 @@
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="17"/>
+      <c r="M25" s="15"/>
       <c r="N25" s="6"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1287,7 +1319,7 @@
       <c r="T25" s="1"/>
     </row>
     <row r="26" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I26" s="19" t="s">
+      <c r="I26" s="17" t="s">
         <v>35</v>
       </c>
       <c r="J26" s="6" t="s">
@@ -1295,7 +1327,7 @@
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="17"/>
+      <c r="M26" s="15"/>
       <c r="N26" s="6"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1305,7 +1337,7 @@
       <c r="T26" s="1"/>
     </row>
     <row r="27" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I27" s="19" t="s">
+      <c r="I27" s="17" t="s">
         <v>34</v>
       </c>
       <c r="J27" s="6" t="s">
@@ -1313,7 +1345,7 @@
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="17"/>
+      <c r="M27" s="15"/>
       <c r="N27" s="6"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -1323,15 +1355,15 @@
       <c r="T27" s="1"/>
     </row>
     <row r="28" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="23" t="s">
+      <c r="J28" s="21" t="s">
         <v>13</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="18"/>
+      <c r="M28" s="16"/>
       <c r="N28" s="7"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1341,10 +1373,10 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="J29" s="21" t="s">
         <v>14</v>
       </c>
       <c r="K29" s="1"/>
@@ -1359,10 +1391,10 @@
       <c r="T29" s="1"/>
     </row>
     <row r="30" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I30" s="22" t="s">
+      <c r="I30" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="21" t="s">
         <v>15</v>
       </c>
       <c r="K30" s="1"/>
@@ -1377,10 +1409,10 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I31" s="22" t="s">
+      <c r="I31" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="23" t="s">
+      <c r="J31" s="21" t="s">
         <v>55</v>
       </c>
       <c r="K31" s="1"/>
@@ -1395,7 +1427,7 @@
       <c r="T31" s="1"/>
     </row>
     <row r="32" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I32" s="20"/>
+      <c r="I32" s="18"/>
       <c r="J32" s="11" t="s">
         <v>51</v>
       </c>
@@ -1411,10 +1443,10 @@
       <c r="T32" s="1"/>
     </row>
     <row r="33" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I33" s="24" t="s">
+      <c r="I33" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J33" s="25" t="s">
+      <c r="J33" s="23" t="s">
         <v>16</v>
       </c>
       <c r="K33" s="1"/>
@@ -1429,10 +1461,10 @@
       <c r="T33" s="1"/>
     </row>
     <row r="34" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I34" s="24" t="s">
+      <c r="I34" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J34" s="25" t="s">
+      <c r="J34" s="23" t="s">
         <v>17</v>
       </c>
       <c r="K34" s="1"/>
@@ -1447,10 +1479,10 @@
       <c r="T34" s="1"/>
     </row>
     <row r="35" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I35" s="24" t="s">
+      <c r="I35" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J35" s="25" t="s">
+      <c r="J35" s="23" t="s">
         <v>18</v>
       </c>
       <c r="K35" s="1"/>
@@ -1465,10 +1497,10 @@
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I36" s="24" t="s">
+      <c r="I36" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="25" t="s">
+      <c r="J36" s="23" t="s">
         <v>19</v>
       </c>
       <c r="K36" s="1"/>
@@ -1483,10 +1515,10 @@
       <c r="T36" s="1"/>
     </row>
     <row r="37" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I37" s="24" t="s">
+      <c r="I37" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J37" s="25" t="s">
+      <c r="J37" s="23" t="s">
         <v>20</v>
       </c>
       <c r="K37" s="1"/>
@@ -1501,10 +1533,10 @@
       <c r="T37" s="1"/>
     </row>
     <row r="38" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I38" s="24" t="s">
+      <c r="I38" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="25" t="s">
+      <c r="J38" s="23" t="s">
         <v>21</v>
       </c>
       <c r="K38" s="1"/>
@@ -1519,7 +1551,7 @@
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I39" s="20"/>
+      <c r="I39" s="18"/>
       <c r="J39" s="11" t="s">
         <v>52</v>
       </c>
@@ -1535,7 +1567,7 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I40" s="21" t="s">
+      <c r="I40" s="19" t="s">
         <v>23</v>
       </c>
       <c r="J40" s="7" t="s">

</xml_diff>

<commit_message>
Now using AFDisp, AFDispH and AFDispV | Trying clustering without filtering records during insertion
</commit_message>
<xml_diff>
--- a/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
+++ b/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\Clustering_Framework\FeatureEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D928030B-B48E-407A-BB0B-5563B7BEE37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CB25476-6DA9-4D13-93BC-D76E2A427BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2792A3-F0C5-48C1-A90B-69EA6F275323}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>Initials</t>
   </si>
@@ -138,24 +138,12 @@
     <t>SSV</t>
   </si>
   <si>
-    <t>SAMi</t>
-  </si>
-  <si>
-    <t>SAMa</t>
-  </si>
-  <si>
     <t>ASA</t>
   </si>
   <si>
     <t>SAT</t>
   </si>
   <si>
-    <t>SDMa</t>
-  </si>
-  <si>
-    <t>SDMi</t>
-  </si>
-  <si>
     <t>SDT</t>
   </si>
   <si>
@@ -163,9 +151,6 @@
   </si>
   <si>
     <t>SC</t>
-  </si>
-  <si>
-    <t>FDA</t>
   </si>
   <si>
     <t>FDT</t>
@@ -277,6 +262,33 @@
   </si>
   <si>
     <t>Average distance between eyes during fixations</t>
+  </si>
+  <si>
+    <t>AFDispH</t>
+  </si>
+  <si>
+    <t>AFDispV</t>
+  </si>
+  <si>
+    <t>Fixation vertical dispersion average</t>
+  </si>
+  <si>
+    <t>Fixation horizontal dispersion average</t>
+  </si>
+  <si>
+    <t>AFDisp</t>
+  </si>
+  <si>
+    <t>SDMax</t>
+  </si>
+  <si>
+    <t>SDMin</t>
+  </si>
+  <si>
+    <t>SAMax</t>
+  </si>
+  <si>
+    <t>SAMin</t>
   </si>
 </sst>
 </file>
@@ -482,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -544,6 +556,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C7A390-9349-4E1E-BAD7-74963176F530}">
-  <dimension ref="I1:T40"/>
+  <dimension ref="I1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,13 +976,13 @@
     <row r="7" spans="9:20" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I7" s="4"/>
       <c r="J7" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -999,15 +1016,15 @@
     <row r="9" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I9" s="10"/>
       <c r="J9" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
@@ -1018,18 +1035,18 @@
     </row>
     <row r="10" spans="9:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1040,7 +1057,7 @@
     </row>
     <row r="11" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I11" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>2</v>
@@ -1048,10 +1065,10 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="24" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1062,7 +1079,7 @@
     </row>
     <row r="12" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I12" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>3</v>
@@ -1070,10 +1087,10 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="24" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1084,7 +1101,7 @@
     </row>
     <row r="13" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I13" s="17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>4</v>
@@ -1092,10 +1109,10 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1106,10 +1123,10 @@
     </row>
     <row r="14" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I14" s="20" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1124,10 +1141,10 @@
     </row>
     <row r="15" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I15" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>58</v>
+        <v>73</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1141,9 +1158,11 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I16" s="18"/>
-      <c r="J16" s="11" t="s">
-        <v>49</v>
+      <c r="I16" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>72</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1158,10 +1177,10 @@
     </row>
     <row r="17" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I17" s="17" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1175,11 +1194,9 @@
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I18" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>5</v>
+      <c r="I18" s="18"/>
+      <c r="J18" s="28" t="s">
+        <v>44</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1193,11 +1210,11 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I19" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>6</v>
+      <c r="I19" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1212,10 +1229,10 @@
     </row>
     <row r="20" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I20" s="17" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1229,11 +1246,11 @@
       <c r="T20" s="1"/>
     </row>
     <row r="21" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I21" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>8</v>
+      <c r="I21" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1247,11 +1264,11 @@
       <c r="T21" s="1"/>
     </row>
     <row r="22" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I22" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>54</v>
+      <c r="I22" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1266,10 +1283,10 @@
     </row>
     <row r="23" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I23" s="17" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1284,10 +1301,10 @@
     </row>
     <row r="24" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I24" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1301,11 +1318,11 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I25" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>10</v>
+      <c r="I25" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1319,11 +1336,11 @@
       <c r="T25" s="1"/>
     </row>
     <row r="26" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>11</v>
+      <c r="J26" s="21" t="s">
+        <v>9</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1341,7 +1358,7 @@
         <v>34</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1354,17 +1371,17 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I28" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J28" s="21" t="s">
-        <v>13</v>
+    <row r="28" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I28" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="7"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="6"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
@@ -1373,16 +1390,16 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I29" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="J29" s="21" t="s">
-        <v>14</v>
+      <c r="I29" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="6"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
@@ -1390,17 +1407,17 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I30" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J30" s="21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="7"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
@@ -1410,10 +1427,10 @@
     </row>
     <row r="31" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I31" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J31" s="21" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1427,9 +1444,11 @@
       <c r="T31" s="1"/>
     </row>
     <row r="32" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I32" s="18"/>
-      <c r="J32" s="11" t="s">
-        <v>51</v>
+      <c r="I32" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>15</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1443,11 +1462,11 @@
       <c r="T32" s="1"/>
     </row>
     <row r="33" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I33" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="J33" s="23" t="s">
-        <v>16</v>
+      <c r="I33" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1461,11 +1480,9 @@
       <c r="T33" s="1"/>
     </row>
     <row r="34" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I34" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J34" s="23" t="s">
-        <v>17</v>
+      <c r="I34" s="18"/>
+      <c r="J34" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1480,10 +1497,10 @@
     </row>
     <row r="35" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I35" s="22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1498,10 +1515,10 @@
     </row>
     <row r="36" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I36" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1516,10 +1533,10 @@
     </row>
     <row r="37" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I37" s="22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1534,10 +1551,10 @@
     </row>
     <row r="38" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I38" s="22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -1551,9 +1568,11 @@
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I39" s="18"/>
-      <c r="J39" s="11" t="s">
-        <v>52</v>
+      <c r="I39" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -1566,12 +1585,12 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I40" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>22</v>
+    <row r="40" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I40" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -1584,6 +1603,40 @@
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
     </row>
+    <row r="41" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I41" s="18"/>
+      <c r="J41" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+    </row>
+    <row r="42" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I42" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Running tests for 2 and 3 features | AUCC working
</commit_message>
<xml_diff>
--- a/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
+++ b/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\Clustering_Framework\FeatureEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CB25476-6DA9-4D13-93BC-D76E2A427BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3EFC45-69ED-4DE9-AF57-16D2488006A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2792A3-F0C5-48C1-A90B-69EA6F275323}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -330,7 +329,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,6 +384,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -494,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -540,9 +545,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -551,16 +553,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C7A390-9349-4E1E-BAD7-74963176F530}">
   <dimension ref="I1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1028,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="25" t="s">
+      <c r="M9" s="29" t="s">
         <v>58</v>
       </c>
       <c r="N9" s="14" t="s">
@@ -1034,7 +1042,7 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="9:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J10" s="6" t="s">
@@ -1042,7 +1050,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="24" t="s">
+      <c r="M10" s="30" t="s">
         <v>60</v>
       </c>
       <c r="N10" s="6" t="s">
@@ -1056,7 +1064,7 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="27" t="s">
         <v>42</v>
       </c>
       <c r="J11" s="6" t="s">
@@ -1064,7 +1072,7 @@
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="30" t="s">
         <v>64</v>
       </c>
       <c r="N11" s="6" t="s">
@@ -1086,7 +1094,7 @@
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="24" t="s">
+      <c r="M12" s="30" t="s">
         <v>65</v>
       </c>
       <c r="N12" s="6" t="s">
@@ -1108,7 +1116,7 @@
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="26" t="s">
+      <c r="M13" s="23" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="6" t="s">
@@ -1122,10 +1130,10 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="20" t="s">
         <v>52</v>
       </c>
       <c r="K14" s="1"/>
@@ -1140,10 +1148,10 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="26" t="s">
         <v>53</v>
       </c>
       <c r="K15" s="1"/>
@@ -1158,10 +1166,10 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="24" t="s">
         <v>72</v>
       </c>
       <c r="K16" s="1"/>
@@ -1176,7 +1184,7 @@
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="27" t="s">
         <v>70</v>
       </c>
       <c r="J17" s="6" t="s">
@@ -1195,7 +1203,7 @@
     </row>
     <row r="18" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="I18" s="18"/>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="25" t="s">
         <v>44</v>
       </c>
       <c r="K18" s="1"/>
@@ -1246,10 +1254,10 @@
       <c r="T20" s="1"/>
     </row>
     <row r="21" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="J21" s="20" t="s">
         <v>6</v>
       </c>
       <c r="K21" s="1"/>
@@ -1300,10 +1308,10 @@
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J24" s="21" t="s">
+      <c r="J24" s="20" t="s">
         <v>49</v>
       </c>
       <c r="K24" s="1"/>
@@ -1318,10 +1326,10 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J25" s="21" t="s">
+      <c r="J25" s="20" t="s">
         <v>51</v>
       </c>
       <c r="K25" s="1"/>
@@ -1336,10 +1344,10 @@
       <c r="T25" s="1"/>
     </row>
     <row r="26" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I26" s="20" t="s">
+      <c r="I26" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="20" t="s">
         <v>9</v>
       </c>
       <c r="K26" s="1"/>
@@ -1354,7 +1362,7 @@
       <c r="T26" s="1"/>
     </row>
     <row r="27" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="27" t="s">
         <v>34</v>
       </c>
       <c r="J27" s="6" t="s">
@@ -1408,10 +1416,10 @@
       <c r="T29" s="1"/>
     </row>
     <row r="30" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I30" s="20" t="s">
+      <c r="I30" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="21" t="s">
+      <c r="J30" s="20" t="s">
         <v>13</v>
       </c>
       <c r="K30" s="1"/>
@@ -1426,10 +1434,10 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I31" s="20" t="s">
+      <c r="I31" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="21" t="s">
+      <c r="J31" s="20" t="s">
         <v>14</v>
       </c>
       <c r="K31" s="1"/>
@@ -1444,10 +1452,10 @@
       <c r="T31" s="1"/>
     </row>
     <row r="32" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I32" s="20" t="s">
+      <c r="I32" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J32" s="21" t="s">
+      <c r="J32" s="20" t="s">
         <v>15</v>
       </c>
       <c r="K32" s="1"/>
@@ -1462,10 +1470,10 @@
       <c r="T32" s="1"/>
     </row>
     <row r="33" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I33" s="20" t="s">
+      <c r="I33" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="21" t="s">
+      <c r="J33" s="20" t="s">
         <v>50</v>
       </c>
       <c r="K33" s="1"/>
@@ -1496,10 +1504,10 @@
       <c r="T34" s="1"/>
     </row>
     <row r="35" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I35" s="22" t="s">
+      <c r="I35" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J35" s="23" t="s">
+      <c r="J35" s="22" t="s">
         <v>16</v>
       </c>
       <c r="K35" s="1"/>
@@ -1514,10 +1522,10 @@
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I36" s="22" t="s">
+      <c r="I36" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="J36" s="22" t="s">
         <v>17</v>
       </c>
       <c r="K36" s="1"/>
@@ -1532,10 +1540,10 @@
       <c r="T36" s="1"/>
     </row>
     <row r="37" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I37" s="22" t="s">
+      <c r="I37" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="23" t="s">
+      <c r="J37" s="22" t="s">
         <v>18</v>
       </c>
       <c r="K37" s="1"/>
@@ -1550,10 +1558,10 @@
       <c r="T37" s="1"/>
     </row>
     <row r="38" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I38" s="22" t="s">
+      <c r="I38" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J38" s="23" t="s">
+      <c r="J38" s="22" t="s">
         <v>19</v>
       </c>
       <c r="K38" s="1"/>
@@ -1568,10 +1576,10 @@
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I39" s="22" t="s">
+      <c r="I39" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J39" s="23" t="s">
+      <c r="J39" s="22" t="s">
         <v>20</v>
       </c>
       <c r="K39" s="1"/>
@@ -1586,10 +1594,10 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="I40" s="22" t="s">
+      <c r="I40" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="J40" s="22" t="s">
         <v>21</v>
       </c>
       <c r="K40" s="1"/>
@@ -1620,7 +1628,7 @@
       <c r="T41" s="1"/>
     </row>
     <row r="42" spans="9:20" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I42" s="19" t="s">
+      <c r="I42" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J42" s="7" t="s">

</xml_diff>

<commit_message>
All best results included (until 265 recordings)
</commit_message>
<xml_diff>
--- a/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
+++ b/Clustering_Framework/FeatureEngineering/Features to Extract.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\Clustering_Framework\FeatureEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3EFC45-69ED-4DE9-AF57-16D2488006A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508E4640-0EBC-424E-BEF2-F1693E46414E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2792A3-F0C5-48C1-A90B-69EA6F275323}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
   <si>
     <t>Initials</t>
   </si>
@@ -289,12 +289,39 @@
   <si>
     <t>SAMin</t>
   </si>
+  <si>
+    <t>ADpFFL</t>
+  </si>
+  <si>
+    <t>ADpFFR</t>
+  </si>
+  <si>
+    <t>Average distance per figure fixation on the left side of the screen</t>
+  </si>
+  <si>
+    <t>Average distance per figure fixation on the right side of the screen</t>
+  </si>
+  <si>
+    <t>ADFF</t>
+  </si>
+  <si>
+    <t>Average distance to first fixations (1º, 11º and 21º)</t>
+  </si>
+  <si>
+    <t>Scan Path Length</t>
+  </si>
+  <si>
+    <t>Maximum of saccade duration</t>
+  </si>
+  <si>
+    <t>Minimum of saccade duration</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,8 +355,15 @@
       <name val="Bahnschrift Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +421,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -569,6 +621,57 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C7A390-9349-4E1E-BAD7-74963176F530}">
-  <dimension ref="I1:T42"/>
+  <dimension ref="I1:T86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="H58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N72" sqref="N72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,10 +1153,10 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="34" t="s">
         <v>61</v>
       </c>
       <c r="O10" s="1"/>
@@ -1129,7 +1232,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="9:20" ht="39" x14ac:dyDescent="0.25">
       <c r="I14" s="19" t="s">
         <v>39</v>
       </c>
@@ -1138,8 +1241,12 @@
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="6"/>
+      <c r="M14" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -1147,7 +1254,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="9:20" ht="39" x14ac:dyDescent="0.25">
       <c r="I15" s="27" t="s">
         <v>73</v>
       </c>
@@ -1156,8 +1263,12 @@
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="6"/>
+      <c r="M15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15" s="32" t="s">
+        <v>81</v>
+      </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -1174,8 +1285,12 @@
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="6"/>
+      <c r="M16" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -1645,6 +1760,312 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
     </row>
+    <row r="45" spans="9:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="9:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I46" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="J46" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I47" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="9:20" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I48" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="J48" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I49" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="J49" s="47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I50" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="J50" s="47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I51" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="J51" s="38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I52" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="J52" s="38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I53" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="J53" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I54" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="J54" s="47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I55" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I56" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="J56" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I57" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="J57" s="47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I58" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="J58" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I59" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="J59" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I60" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="J60" s="47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="9:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I61" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="J61" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I62" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="J62" s="37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I63" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="J63" s="43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I64" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="J64" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I65" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="J65" s="44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I66" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="J66" s="44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="9:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I67" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="J67" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="9:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I71" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="J71" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I72" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="J72" s="37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I73" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="J73" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I74" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="J74" s="38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="75" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I75" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="J75" s="38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I76" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="J76" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I77" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J77" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I78" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="J78" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I79" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="J79" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="9:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I80" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="J80" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I81" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J81" s="37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I82" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="J82" s="43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I83" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="J83" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I84" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="J84" s="44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="9:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="I85" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="J85" s="44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="9:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I86" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="J86" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>